<commit_message>
Update sample data to support up to 100 students
</commit_message>
<xml_diff>
--- a/sample_students.xlsx
+++ b/sample_students.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C81"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -523,9 +523,779 @@
         <v>jack.anderson@student.edu</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>Kevin Lee</v>
+      </c>
+      <c r="B12" t="str">
+        <v>REG011</v>
+      </c>
+      <c r="C12" t="str">
+        <v>kevin.lee@student.edu</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>Laura Garcia</v>
+      </c>
+      <c r="B13" t="str">
+        <v>REG012</v>
+      </c>
+      <c r="C13" t="str">
+        <v>laura.garcia@student.edu</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>Mike Chen</v>
+      </c>
+      <c r="B14" t="str">
+        <v>REG013</v>
+      </c>
+      <c r="C14" t="str">
+        <v>mike.chen@student.edu</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>Nancy Patel</v>
+      </c>
+      <c r="B15" t="str">
+        <v>REG014</v>
+      </c>
+      <c r="C15" t="str">
+        <v>nancy.patel@student.edu</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>Oliver Kim</v>
+      </c>
+      <c r="B16" t="str">
+        <v>REG015</v>
+      </c>
+      <c r="C16" t="str">
+        <v>oliver.kim@student.edu</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>Paula Rodriguez</v>
+      </c>
+      <c r="B17" t="str">
+        <v>REG016</v>
+      </c>
+      <c r="C17" t="str">
+        <v>paula.rodriguez@student.edu</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>Quinn Thompson</v>
+      </c>
+      <c r="B18" t="str">
+        <v>REG017</v>
+      </c>
+      <c r="C18" t="str">
+        <v>quinn.thompson@student.edu</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>Rachel Nguyen</v>
+      </c>
+      <c r="B19" t="str">
+        <v>REG018</v>
+      </c>
+      <c r="C19" t="str">
+        <v>rachel.nguyen@student.edu</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>Steven Davis</v>
+      </c>
+      <c r="B20" t="str">
+        <v>REG019</v>
+      </c>
+      <c r="C20" t="str">
+        <v>steven.davis@student.edu</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>Tina Martinez</v>
+      </c>
+      <c r="B21" t="str">
+        <v>REG020</v>
+      </c>
+      <c r="C21" t="str">
+        <v>tina.martinez@student.edu</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>Ursula Wilson</v>
+      </c>
+      <c r="B22" t="str">
+        <v>REG021</v>
+      </c>
+      <c r="C22" t="str">
+        <v>ursula.wilson@student.edu</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>Victor Brown</v>
+      </c>
+      <c r="B23" t="str">
+        <v>REG022</v>
+      </c>
+      <c r="C23" t="str">
+        <v>victor.brown@student.edu</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>Wendy Taylor</v>
+      </c>
+      <c r="B24" t="str">
+        <v>REG023</v>
+      </c>
+      <c r="C24" t="str">
+        <v>wendy.taylor@student.edu</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>Xavier Johnson</v>
+      </c>
+      <c r="B25" t="str">
+        <v>REG024</v>
+      </c>
+      <c r="C25" t="str">
+        <v>xavier.johnson@student.edu</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>Yara Smith</v>
+      </c>
+      <c r="B26" t="str">
+        <v>REG025</v>
+      </c>
+      <c r="C26" t="str">
+        <v>yara.smith@student.edu</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>Zachary Williams</v>
+      </c>
+      <c r="B27" t="str">
+        <v>REG026</v>
+      </c>
+      <c r="C27" t="str">
+        <v>zachary.williams@student.edu</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>Aaron Brown</v>
+      </c>
+      <c r="B28" t="str">
+        <v>REG027</v>
+      </c>
+      <c r="C28" t="str">
+        <v>aaron.brown@student.edu</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>Bella Davis</v>
+      </c>
+      <c r="B29" t="str">
+        <v>REG028</v>
+      </c>
+      <c r="C29" t="str">
+        <v>bella.davis@student.edu</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>Caleb Miller</v>
+      </c>
+      <c r="B30" t="str">
+        <v>REG029</v>
+      </c>
+      <c r="C30" t="str">
+        <v>caleb.miller@student.edu</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>Diana Wilson</v>
+      </c>
+      <c r="B31" t="str">
+        <v>REG030</v>
+      </c>
+      <c r="C31" t="str">
+        <v>diana.wilson@student.edu</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>Ethan Moore</v>
+      </c>
+      <c r="B32" t="str">
+        <v>REG031</v>
+      </c>
+      <c r="C32" t="str">
+        <v>ethan.moore@student.edu</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>Fiona Taylor</v>
+      </c>
+      <c r="B33" t="str">
+        <v>REG032</v>
+      </c>
+      <c r="C33" t="str">
+        <v>fiona.taylor@student.edu</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>Gavin Anderson</v>
+      </c>
+      <c r="B34" t="str">
+        <v>REG033</v>
+      </c>
+      <c r="C34" t="str">
+        <v>gavin.anderson@student.edu</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>Hannah Lee</v>
+      </c>
+      <c r="B35" t="str">
+        <v>REG034</v>
+      </c>
+      <c r="C35" t="str">
+        <v>hannah.lee@student.edu</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>Ian Garcia</v>
+      </c>
+      <c r="B36" t="str">
+        <v>REG035</v>
+      </c>
+      <c r="C36" t="str">
+        <v>ian.garcia@student.edu</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>Julia Chen</v>
+      </c>
+      <c r="B37" t="str">
+        <v>REG036</v>
+      </c>
+      <c r="C37" t="str">
+        <v>julia.chen@student.edu</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>Kyle Patel</v>
+      </c>
+      <c r="B38" t="str">
+        <v>REG037</v>
+      </c>
+      <c r="C38" t="str">
+        <v>kyle.patel@student.edu</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>Lily Kim</v>
+      </c>
+      <c r="B39" t="str">
+        <v>REG038</v>
+      </c>
+      <c r="C39" t="str">
+        <v>lily.kim@student.edu</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>Mason Rodriguez</v>
+      </c>
+      <c r="B40" t="str">
+        <v>REG039</v>
+      </c>
+      <c r="C40" t="str">
+        <v>mason.rodriguez@student.edu</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>Nora Thompson</v>
+      </c>
+      <c r="B41" t="str">
+        <v>REG040</v>
+      </c>
+      <c r="C41" t="str">
+        <v>nora.thompson@student.edu</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>Owen Nguyen</v>
+      </c>
+      <c r="B42" t="str">
+        <v>REG041</v>
+      </c>
+      <c r="C42" t="str">
+        <v>owen.nguyen@student.edu</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>Piper Davis</v>
+      </c>
+      <c r="B43" t="str">
+        <v>REG042</v>
+      </c>
+      <c r="C43" t="str">
+        <v>piper.davis@student.edu</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>Quincy Martinez</v>
+      </c>
+      <c r="B44" t="str">
+        <v>REG043</v>
+      </c>
+      <c r="C44" t="str">
+        <v>quincy.martinez@student.edu</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>Riley Wilson</v>
+      </c>
+      <c r="B45" t="str">
+        <v>REG044</v>
+      </c>
+      <c r="C45" t="str">
+        <v>riley.wilson@student.edu</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>Samantha Brown</v>
+      </c>
+      <c r="B46" t="str">
+        <v>REG045</v>
+      </c>
+      <c r="C46" t="str">
+        <v>samantha.brown@student.edu</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>Tyler Taylor</v>
+      </c>
+      <c r="B47" t="str">
+        <v>REG046</v>
+      </c>
+      <c r="C47" t="str">
+        <v>tyler.taylor@student.edu</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>Uma Johnson</v>
+      </c>
+      <c r="B48" t="str">
+        <v>REG047</v>
+      </c>
+      <c r="C48" t="str">
+        <v>uma.johnson@student.edu</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>Vincent Smith</v>
+      </c>
+      <c r="B49" t="str">
+        <v>REG048</v>
+      </c>
+      <c r="C49" t="str">
+        <v>vincent.smith@student.edu</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>Willow Williams</v>
+      </c>
+      <c r="B50" t="str">
+        <v>REG049</v>
+      </c>
+      <c r="C50" t="str">
+        <v>willow.williams@student.edu</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>Xander Brown</v>
+      </c>
+      <c r="B51" t="str">
+        <v>REG050</v>
+      </c>
+      <c r="C51" t="str">
+        <v>xander.brown@student.edu</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>Yasmine Davis</v>
+      </c>
+      <c r="B52" t="str">
+        <v>REG051</v>
+      </c>
+      <c r="C52" t="str">
+        <v>yasmine.davis@student.edu</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>Zoe Miller</v>
+      </c>
+      <c r="B53" t="str">
+        <v>REG052</v>
+      </c>
+      <c r="C53" t="str">
+        <v>zoe.miller@student.edu</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>Adrian Wilson</v>
+      </c>
+      <c r="B54" t="str">
+        <v>REG053</v>
+      </c>
+      <c r="C54" t="str">
+        <v>adrian.wilson@student.edu</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>Brooke Moore</v>
+      </c>
+      <c r="B55" t="str">
+        <v>REG054</v>
+      </c>
+      <c r="C55" t="str">
+        <v>brooke.moore@student.edu</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>Carter Taylor</v>
+      </c>
+      <c r="B56" t="str">
+        <v>REG055</v>
+      </c>
+      <c r="C56" t="str">
+        <v>carter.taylor@student.edu</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>Delilah Anderson</v>
+      </c>
+      <c r="B57" t="str">
+        <v>REG056</v>
+      </c>
+      <c r="C57" t="str">
+        <v>delilah.anderson@student.edu</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>Eli Lee</v>
+      </c>
+      <c r="B58" t="str">
+        <v>REG057</v>
+      </c>
+      <c r="C58" t="str">
+        <v>eli.lee@student.edu</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>Faith Garcia</v>
+      </c>
+      <c r="B59" t="str">
+        <v>REG058</v>
+      </c>
+      <c r="C59" t="str">
+        <v>faith.garcia@student.edu</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>Gideon Chen</v>
+      </c>
+      <c r="B60" t="str">
+        <v>REG059</v>
+      </c>
+      <c r="C60" t="str">
+        <v>gideon.chen@student.edu</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>Harper Patel</v>
+      </c>
+      <c r="B61" t="str">
+        <v>REG060</v>
+      </c>
+      <c r="C61" t="str">
+        <v>harper.patel@student.edu</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v>Isaac Kim</v>
+      </c>
+      <c r="B62" t="str">
+        <v>REG061</v>
+      </c>
+      <c r="C62" t="str">
+        <v>isaac.kim@student.edu</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v>Jasmine Rodriguez</v>
+      </c>
+      <c r="B63" t="str">
+        <v>REG062</v>
+      </c>
+      <c r="C63" t="str">
+        <v>jasmine.rodriguez@student.edu</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v>Kai Thompson</v>
+      </c>
+      <c r="B64" t="str">
+        <v>REG063</v>
+      </c>
+      <c r="C64" t="str">
+        <v>kai.thompson@student.edu</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v>Luna Nguyen</v>
+      </c>
+      <c r="B65" t="str">
+        <v>REG064</v>
+      </c>
+      <c r="C65" t="str">
+        <v>luna.nguyen@student.edu</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="str">
+        <v>Milo Davis</v>
+      </c>
+      <c r="B66" t="str">
+        <v>REG065</v>
+      </c>
+      <c r="C66" t="str">
+        <v>milo.davis@student.edu</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="str">
+        <v>Nova Martinez</v>
+      </c>
+      <c r="B67" t="str">
+        <v>REG066</v>
+      </c>
+      <c r="C67" t="str">
+        <v>nova.martinez@student.edu</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="str">
+        <v>Oscar Wilson</v>
+      </c>
+      <c r="B68" t="str">
+        <v>REG067</v>
+      </c>
+      <c r="C68" t="str">
+        <v>oscar.wilson@student.edu</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="str">
+        <v>Penelope Brown</v>
+      </c>
+      <c r="B69" t="str">
+        <v>REG068</v>
+      </c>
+      <c r="C69" t="str">
+        <v>penelope.brown@student.edu</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="str">
+        <v>Quinn Taylor</v>
+      </c>
+      <c r="B70" t="str">
+        <v>REG069</v>
+      </c>
+      <c r="C70" t="str">
+        <v>quinn.taylor@student.edu</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="str">
+        <v>Roman Johnson</v>
+      </c>
+      <c r="B71" t="str">
+        <v>REG070</v>
+      </c>
+      <c r="C71" t="str">
+        <v>roman.johnson@student.edu</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="str">
+        <v>Scarlett Smith</v>
+      </c>
+      <c r="B72" t="str">
+        <v>REG071</v>
+      </c>
+      <c r="C72" t="str">
+        <v>scarlett.smith@student.edu</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>Theo Williams</v>
+      </c>
+      <c r="B73" t="str">
+        <v>REG072</v>
+      </c>
+      <c r="C73" t="str">
+        <v>theo.williams@student.edu</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="str">
+        <v>Violet Brown</v>
+      </c>
+      <c r="B74" t="str">
+        <v>REG073</v>
+      </c>
+      <c r="C74" t="str">
+        <v>violet.brown@student.edu</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="str">
+        <v>Wyatt Davis</v>
+      </c>
+      <c r="B75" t="str">
+        <v>REG074</v>
+      </c>
+      <c r="C75" t="str">
+        <v>wyatt.davis@student.edu</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v>Xanthe Miller</v>
+      </c>
+      <c r="B76" t="str">
+        <v>REG075</v>
+      </c>
+      <c r="C76" t="str">
+        <v>xanthe.miller@student.edu</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="str">
+        <v>Yusuf Wilson</v>
+      </c>
+      <c r="B77" t="str">
+        <v>REG076</v>
+      </c>
+      <c r="C77" t="str">
+        <v>yusuf.wilson@student.edu</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="str">
+        <v>Zara Moore</v>
+      </c>
+      <c r="B78" t="str">
+        <v>REG077</v>
+      </c>
+      <c r="C78" t="str">
+        <v>zara.moore@student.edu</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="str">
+        <v>Asher Taylor</v>
+      </c>
+      <c r="B79" t="str">
+        <v>REG078</v>
+      </c>
+      <c r="C79" t="str">
+        <v>asher.taylor@student.edu</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="str">
+        <v>Bailey Anderson</v>
+      </c>
+      <c r="B80" t="str">
+        <v>REG079</v>
+      </c>
+      <c r="C80" t="str">
+        <v>bailey.anderson@student.edu</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="str">
+        <v>Caden Lee</v>
+      </c>
+      <c r="B81" t="str">
+        <v>REG080</v>
+      </c>
+      <c r="C81" t="str">
+        <v>caden.lee@student.edu</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C81"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Switch to SQLite database
</commit_message>
<xml_diff>
--- a/sample_students.xlsx
+++ b/sample_students.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C81"/>
+  <dimension ref="A1:C101"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1293,9 +1293,229 @@
         <v>caden.lee@student.edu</v>
       </c>
     </row>
+    <row r="82">
+      <c r="A82" t="str">
+        <v>Daniel Garcia</v>
+      </c>
+      <c r="B82" t="str">
+        <v>REG081</v>
+      </c>
+      <c r="C82" t="str">
+        <v>daniel.garcia@student.edu</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="str">
+        <v>Elena Patel</v>
+      </c>
+      <c r="B83" t="str">
+        <v>REG082</v>
+      </c>
+      <c r="C83" t="str">
+        <v>elena.patel@student.edu</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="str">
+        <v>Felix Kim</v>
+      </c>
+      <c r="B84" t="str">
+        <v>REG083</v>
+      </c>
+      <c r="C84" t="str">
+        <v>felix.kim@student.edu</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="str">
+        <v>Gabriella Rodriguez</v>
+      </c>
+      <c r="B85" t="str">
+        <v>REG084</v>
+      </c>
+      <c r="C85" t="str">
+        <v>gabriella.rodriguez@student.edu</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="str">
+        <v>Hunter Thompson</v>
+      </c>
+      <c r="B86" t="str">
+        <v>REG085</v>
+      </c>
+      <c r="C86" t="str">
+        <v>hunter.thompson@student.edu</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="str">
+        <v>Isabella Nguyen</v>
+      </c>
+      <c r="B87" t="str">
+        <v>REG086</v>
+      </c>
+      <c r="C87" t="str">
+        <v>isabella.nguyen@student.edu</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="str">
+        <v>Julian Davis</v>
+      </c>
+      <c r="B88" t="str">
+        <v>REG087</v>
+      </c>
+      <c r="C88" t="str">
+        <v>julian.davis@student.edu</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="str">
+        <v>Katherine Martinez</v>
+      </c>
+      <c r="B89" t="str">
+        <v>REG088</v>
+      </c>
+      <c r="C89" t="str">
+        <v>katherine.martinez@student.edu</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="str">
+        <v>Liam Wilson</v>
+      </c>
+      <c r="B90" t="str">
+        <v>REG089</v>
+      </c>
+      <c r="C90" t="str">
+        <v>liam.wilson@student.edu</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="str">
+        <v>Maya Brown</v>
+      </c>
+      <c r="B91" t="str">
+        <v>REG090</v>
+      </c>
+      <c r="C91" t="str">
+        <v>maya.brown@student.edu</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="str">
+        <v>Nathan Taylor</v>
+      </c>
+      <c r="B92" t="str">
+        <v>REG091</v>
+      </c>
+      <c r="C92" t="str">
+        <v>nathan.taylor@student.edu</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="str">
+        <v>Olivia Johnson</v>
+      </c>
+      <c r="B93" t="str">
+        <v>REG092</v>
+      </c>
+      <c r="C93" t="str">
+        <v>olivia.johnson@student.edu</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="str">
+        <v>Parker Smith</v>
+      </c>
+      <c r="B94" t="str">
+        <v>REG093</v>
+      </c>
+      <c r="C94" t="str">
+        <v>parker.smith@student.edu</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="str">
+        <v>Quinn Williams</v>
+      </c>
+      <c r="B95" t="str">
+        <v>REG094</v>
+      </c>
+      <c r="C95" t="str">
+        <v>quinn.williams@student.edu</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="str">
+        <v>Ryan Brown</v>
+      </c>
+      <c r="B96" t="str">
+        <v>REG095</v>
+      </c>
+      <c r="C96" t="str">
+        <v>ryan.brown@student.edu</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="str">
+        <v>Sophia Davis</v>
+      </c>
+      <c r="B97" t="str">
+        <v>REG096</v>
+      </c>
+      <c r="C97" t="str">
+        <v>sophia.davis@student.edu</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="str">
+        <v>Tristan Miller</v>
+      </c>
+      <c r="B98" t="str">
+        <v>REG097</v>
+      </c>
+      <c r="C98" t="str">
+        <v>tristan.miller@student.edu</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="str">
+        <v>Ulysses Wilson</v>
+      </c>
+      <c r="B99" t="str">
+        <v>REG098</v>
+      </c>
+      <c r="C99" t="str">
+        <v>ulysses.wilson@student.edu</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="str">
+        <v>Victoria Moore</v>
+      </c>
+      <c r="B100" t="str">
+        <v>REG099</v>
+      </c>
+      <c r="C100" t="str">
+        <v>victoria.moore@student.edu</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="str">
+        <v>William Taylor</v>
+      </c>
+      <c r="B101" t="str">
+        <v>REG100</v>
+      </c>
+      <c r="C101" t="str">
+        <v>william.taylor@student.edu</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C81"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C101"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>